<commit_message>
- Adicionada a biblioteca ClosedXML; - Adicionado uma tabela de resultados utilizando planilha excel.
</commit_message>
<xml_diff>
--- a/game/results/results.xlsx
+++ b/game/results/results.xlsx
@@ -595,6 +595,14 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
+    <x:row r="28" spans="1:2">
+      <x:c r="A28" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="B28" s="0">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>